<commit_message>
chore: change to static to static document
</commit_message>
<xml_diff>
--- a/simple1.xlsx
+++ b/simple1.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Staff" sheetId="1" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -67,10 +67,10 @@
     <t>Fong Zu Rong</t>
   </si>
   <si>
-    <t>wefwefwefw</t>
-  </si>
-  <si>
-    <t>08/22/2023 04:07:15 PM</t>
+    <t>Poekoas</t>
+  </si>
+  <si>
+    <t>08/22/2023 04:15:53 PM</t>
   </si>
 </sst>
 </file>

</xml_diff>